<commit_message>
Fix: Correctly handle Daily Lotto bonus numbers.  The script removes incorrectly assigned bonus numbers from Daily Lotto results in the database.
Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 4849bf2d-2ea2-4878-9bf3-daf806bf05dd
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/45399ea3-630c-4463-8e3d-edea73bb30a7/36d4d2aa-e6b6-4bb6-be0a-bc90bd96c011.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Snap_lotto True Numbers and results .xlsx
+++ b/attached_assets/Snap_lotto True Numbers and results .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ef28d14e5ba0b5e9/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96A4B565-5D97-4C3B-BD23-16A6E5E3C3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{96A4B565-5D97-4C3B-BD23-16A6E5E3C3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EFBC5CE-B53B-4E9C-ABF1-26A5A1AD0E10}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{6C370565-C7DA-47FD-B436-DC0A943DF295}"/>
   </bookViews>
@@ -877,12 +877,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423038D3-907C-4384-A57A-97AA890F912B}">
   <dimension ref="A1:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6328125" customWidth="1"/>
   </cols>
@@ -4579,7 +4581,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>2</v>
       </c>

</xml_diff>